<commit_message>
fix bug Duyên nói
</commit_message>
<xml_diff>
--- a/TimeCard/TimeCard/Temp/LỊCH SỬ CHẤM CÔNG THÁNG 12 NĂM 2020.xlsx
+++ b/TimeCard/TimeCard/Temp/LỊCH SỬ CHẤM CÔNG THÁNG 12 NĂM 2020.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <x:si>
     <x:t>CHI TIẾT CHẤM CÔNG CỦA PGDKQLTD2</x:t>
   </x:si>
@@ -88,6 +88,15 @@
   </x:si>
   <x:si>
     <x:t>Thử nghiệm app</x:t>
+  </x:si>
+  <x:si>
+    <x:t>abc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>def</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> </x:t>
   </x:si>
   <x:si>
     <x:t>CHI TIẾT CHẤM CÔNG CỦA PHUONGLNL</x:t>
@@ -263,7 +272,7 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="13">
+  <x:cellStyleXfs count="14">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -301,8 +310,11 @@
     <x:xf numFmtId="0" fontId="4" fillId="4" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="46" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="21">
+  <x:cellXfs count="22">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -357,6 +369,10 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="46" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -688,7 +704,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:13" customFormat="1" ht="17.4" customHeight="1">
       <x:c r="B2" s="11" t="s">
-        <x:v>25</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C2" s="11" t="s"/>
       <x:c r="D2" s="11" t="s"/>
@@ -1308,7 +1324,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:13" customFormat="1" ht="17.4" customHeight="1">
       <x:c r="B2" s="11" t="s">
-        <x:v>26</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C2" s="11" t="s"/>
       <x:c r="D2" s="11" t="s"/>
@@ -1928,7 +1944,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:13" customFormat="1" ht="17.4" customHeight="1">
       <x:c r="B2" s="11" t="s">
-        <x:v>27</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C2" s="11" t="s"/>
       <x:c r="D2" s="11" t="s"/>
@@ -2548,7 +2564,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:13" customFormat="1" ht="17.4" customHeight="1">
       <x:c r="B2" s="11" t="s">
-        <x:v>28</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C2" s="11" t="s"/>
       <x:c r="D2" s="11" t="s"/>
@@ -3168,7 +3184,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:13" customFormat="1" ht="17.4" customHeight="1">
       <x:c r="B2" s="11" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C2" s="11" t="s"/>
       <x:c r="D2" s="11" t="s"/>
@@ -3788,7 +3804,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:13" customFormat="1" ht="17.4" customHeight="1">
       <x:c r="B2" s="11" t="s">
-        <x:v>30</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C2" s="11" t="s"/>
       <x:c r="D2" s="11" t="s"/>
@@ -4408,7 +4424,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:13" customFormat="1" ht="17.4" customHeight="1">
       <x:c r="B2" s="11" t="s">
-        <x:v>31</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C2" s="11" t="s"/>
       <x:c r="D2" s="11" t="s"/>
@@ -5845,7 +5861,9 @@
         <x:v>440</x:v>
       </x:c>
       <x:c r="G12" s="19" t="s"/>
-      <x:c r="H12" s="19" t="s"/>
+      <x:c r="H12" s="18" t="s">
+        <x:v>14</x:v>
+      </x:c>
       <x:c r="I12" s="19" t="n">
         <x:v>98</x:v>
       </x:c>
@@ -5882,7 +5900,7 @@
         <x:v>0.399305555555556</x:v>
       </x:c>
       <x:c r="D14" s="17" t="n">
-        <x:v>0.399305555555556</x:v>
+        <x:v>0.774305555555555</x:v>
       </x:c>
       <x:c r="E14" s="18" t="s">
         <x:v>14</x:v>
@@ -5891,11 +5909,9 @@
         <x:v>94</x:v>
       </x:c>
       <x:c r="G14" s="19" t="s"/>
-      <x:c r="H14" s="18" t="s">
-        <x:v>14</x:v>
-      </x:c>
+      <x:c r="H14" s="19" t="s"/>
       <x:c r="I14" s="19" t="n">
-        <x:v>444</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="J14" s="19" t="s">
         <x:v>17</x:v>
@@ -6005,20 +6021,36 @@
       <x:c r="M20" s="10" t="s"/>
     </x:row>
     <x:row r="21" spans="1:13">
-      <x:c r="B21" s="14">
+      <x:c r="B21" s="16">
         <x:v>44183</x:v>
       </x:c>
-      <x:c r="C21" s="3" t="s"/>
-      <x:c r="D21" s="3" t="s"/>
-      <x:c r="E21" s="3" t="s"/>
-      <x:c r="F21" s="3" t="s"/>
-      <x:c r="G21" s="3" t="s"/>
-      <x:c r="H21" s="3" t="s"/>
-      <x:c r="I21" s="3" t="s"/>
-      <x:c r="J21" s="3" t="s"/>
-      <x:c r="K21" s="3" t="s"/>
-      <x:c r="L21" s="10" t="s"/>
-      <x:c r="M21" s="10" t="s"/>
+      <x:c r="C21" s="17" t="n">
+        <x:v>0.38125</x:v>
+      </x:c>
+      <x:c r="D21" s="17" t="n">
+        <x:v>0.75625</x:v>
+      </x:c>
+      <x:c r="E21" s="18" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F21" s="19" t="n">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="G21" s="19" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="H21" s="19" t="s"/>
+      <x:c r="I21" s="19" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J21" s="19" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="K21" s="19" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="L21" s="20" t="s"/>
+      <x:c r="M21" s="20" t="s"/>
     </x:row>
     <x:row r="22" spans="1:13">
       <x:c r="B22" s="14">
@@ -6231,21 +6263,21 @@
     <x:row r="35" spans="1:13">
       <x:c r="B35" s="15" t="s"/>
       <x:c r="C35" s="15" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D35" s="15" t="s"/>
       <x:c r="E35" s="15" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="F35" s="15" t="n">
-        <x:v>534</x:v>
+        <x:v>602</x:v>
       </x:c>
       <x:c r="G35" s="15" t="s"/>
       <x:c r="H35" s="15" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="I35" s="15" t="n">
-        <x:v>542</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="J35" s="15" t="s"/>
       <x:c r="K35" s="15" t="s"/>
@@ -6300,7 +6332,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:13" customFormat="1" ht="17.4" customHeight="1">
       <x:c r="B2" s="11" t="s">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C2" s="11" t="s"/>
       <x:c r="D2" s="11" t="s"/>
@@ -6501,7 +6533,7 @@
       </x:c>
       <x:c r="J12" s="19" t="s"/>
       <x:c r="K12" s="19" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="L12" s="20" t="s">
         <x:v>16</x:v>
@@ -6545,7 +6577,7 @@
       </x:c>
       <x:c r="J14" s="19" t="s"/>
       <x:c r="K14" s="19" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="L14" s="20" t="s">
         <x:v>16</x:v>
@@ -6553,30 +6585,30 @@
       <x:c r="M14" s="20" t="s"/>
     </x:row>
     <x:row r="15" spans="1:13">
-      <x:c r="B15" s="16">
+      <x:c r="B15" s="14">
         <x:v>44177</x:v>
       </x:c>
-      <x:c r="C15" s="17" t="n">
-        <x:v>0.390277777777778</x:v>
-      </x:c>
-      <x:c r="D15" s="19" t="s"/>
-      <x:c r="E15" s="18" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="F15" s="19" t="n">
-        <x:v>81</x:v>
-      </x:c>
-      <x:c r="G15" s="19" t="s"/>
-      <x:c r="H15" s="19" t="s"/>
-      <x:c r="I15" s="19" t="n">
+      <x:c r="C15" s="21" t="n">
+        <x:v>0.306944444444444</x:v>
+      </x:c>
+      <x:c r="D15" s="21" t="n">
+        <x:v>0.515277777777778</x:v>
+      </x:c>
+      <x:c r="E15" s="3" t="s"/>
+      <x:c r="F15" s="3" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J15" s="19" t="s"/>
-      <x:c r="K15" s="19" t="s"/>
-      <x:c r="L15" s="20" t="s">
+      <x:c r="G15" s="3" t="s"/>
+      <x:c r="H15" s="3" t="s"/>
+      <x:c r="I15" s="3" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J15" s="3" t="s"/>
+      <x:c r="K15" s="3" t="s"/>
+      <x:c r="L15" s="10" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="M15" s="20" t="s"/>
+      <x:c r="M15" s="10" t="s"/>
     </x:row>
     <x:row r="16" spans="1:13">
       <x:c r="B16" s="14">
@@ -6595,20 +6627,32 @@
       <x:c r="M16" s="10" t="s"/>
     </x:row>
     <x:row r="17" spans="1:13">
-      <x:c r="B17" s="14">
+      <x:c r="B17" s="16">
         <x:v>44179</x:v>
       </x:c>
-      <x:c r="C17" s="3" t="s"/>
-      <x:c r="D17" s="3" t="s"/>
-      <x:c r="E17" s="3" t="s"/>
-      <x:c r="F17" s="3" t="s"/>
-      <x:c r="G17" s="3" t="s"/>
-      <x:c r="H17" s="3" t="s"/>
-      <x:c r="I17" s="3" t="s"/>
-      <x:c r="J17" s="3" t="s"/>
-      <x:c r="K17" s="3" t="s"/>
-      <x:c r="L17" s="10" t="s"/>
-      <x:c r="M17" s="10" t="s"/>
+      <x:c r="C17" s="17" t="n">
+        <x:v>0.345138888888889</x:v>
+      </x:c>
+      <x:c r="D17" s="19" t="s"/>
+      <x:c r="E17" s="18" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F17" s="19" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="G17" s="19" t="s"/>
+      <x:c r="H17" s="19" t="s"/>
+      <x:c r="I17" s="19" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J17" s="19" t="s"/>
+      <x:c r="K17" s="19" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="L17" s="20" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="M17" s="20" t="s"/>
     </x:row>
     <x:row r="18" spans="1:13">
       <x:c r="B18" s="14">
@@ -6659,20 +6703,30 @@
       <x:c r="M20" s="10" t="s"/>
     </x:row>
     <x:row r="21" spans="1:13">
-      <x:c r="B21" s="14">
+      <x:c r="B21" s="16">
         <x:v>44183</x:v>
       </x:c>
-      <x:c r="C21" s="3" t="s"/>
-      <x:c r="D21" s="3" t="s"/>
-      <x:c r="E21" s="3" t="s"/>
-      <x:c r="F21" s="3" t="s"/>
-      <x:c r="G21" s="3" t="s"/>
-      <x:c r="H21" s="3" t="s"/>
-      <x:c r="I21" s="3" t="s"/>
-      <x:c r="J21" s="3" t="s"/>
-      <x:c r="K21" s="3" t="s"/>
-      <x:c r="L21" s="10" t="s"/>
-      <x:c r="M21" s="10" t="s"/>
+      <x:c r="C21" s="17" t="n">
+        <x:v>0.336805555555556</x:v>
+      </x:c>
+      <x:c r="D21" s="19" t="s"/>
+      <x:c r="E21" s="18" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F21" s="19" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="G21" s="19" t="s"/>
+      <x:c r="H21" s="19" t="s"/>
+      <x:c r="I21" s="19" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J21" s="19" t="s"/>
+      <x:c r="K21" s="19" t="s"/>
+      <x:c r="L21" s="20" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="M21" s="20" t="s"/>
     </x:row>
     <x:row r="22" spans="1:13">
       <x:c r="B22" s="14">
@@ -6885,14 +6939,14 @@
     <x:row r="35" spans="1:13">
       <x:c r="B35" s="15" t="s"/>
       <x:c r="C35" s="15" t="n">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="D35" s="15" t="s"/>
       <x:c r="E35" s="15" t="n">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="F35" s="15" t="n">
-        <x:v>604</x:v>
+        <x:v>543</x:v>
       </x:c>
       <x:c r="G35" s="15" t="s"/>
       <x:c r="H35" s="15" t="n">
@@ -6954,7 +7008,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:13" customFormat="1" ht="17.4" customHeight="1">
       <x:c r="B2" s="11" t="s">
-        <x:v>20</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C2" s="11" t="s"/>
       <x:c r="D2" s="11" t="s"/>
@@ -7574,7 +7628,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:13" customFormat="1" ht="17.4" customHeight="1">
       <x:c r="B2" s="11" t="s">
-        <x:v>21</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C2" s="11" t="s"/>
       <x:c r="D2" s="11" t="s"/>
@@ -8194,7 +8248,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:13" customFormat="1" ht="17.4" customHeight="1">
       <x:c r="B2" s="11" t="s">
-        <x:v>22</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C2" s="11" t="s"/>
       <x:c r="D2" s="11" t="s"/>
@@ -8814,7 +8868,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:13" customFormat="1" ht="17.4" customHeight="1">
       <x:c r="B2" s="11" t="s">
-        <x:v>23</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C2" s="11" t="s"/>
       <x:c r="D2" s="11" t="s"/>
@@ -9434,7 +9488,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:13" customFormat="1" ht="17.4" customHeight="1">
       <x:c r="B2" s="11" t="s">
-        <x:v>24</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C2" s="11" t="s"/>
       <x:c r="D2" s="11" t="s"/>

</xml_diff>